<commit_message>
Adjustment for MS Excel
</commit_message>
<xml_diff>
--- a/Assignment 1.xlsx
+++ b/Assignment 1.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="10" documentId="11_D258262CC2B2CBD90605945EC74F8981D2BE7756" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA6BE6B0-FC1A-4379-A00A-72AFD439D3B9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -1169,17 +1169,17 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1221,6 +1221,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1526,7 +1530,7 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -1626,8 +1630,8 @@
   </sheetPr>
   <dimension ref="A1:H150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1698,7 +1702,7 @@
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" ht="13.2">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="45" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -1710,11 +1714,11 @@
       <c r="D4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="46"/>
-      <c r="G4" s="47" t="s">
+      <c r="F4" s="47"/>
+      <c r="G4" s="46" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="13"/>
@@ -1786,7 +1790,7 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" ht="26.4">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="45" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -1798,13 +1802,13 @@
       <c r="D9" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="47" t="s">
+      <c r="G9" s="46" t="s">
         <v>45</v>
       </c>
       <c r="H9" s="13"/>
@@ -2939,7 +2943,7 @@
     <row r="61" spans="1:8" ht="15.6" hidden="1">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
-      <c r="C61" s="45"/>
+      <c r="C61" s="48"/>
       <c r="D61" s="36"/>
       <c r="E61" s="36"/>
       <c r="F61" s="36"/>
@@ -2969,7 +2973,7 @@
     <row r="64" spans="1:8" ht="15.6" hidden="1">
       <c r="A64" s="8"/>
       <c r="B64" s="8"/>
-      <c r="C64" s="45"/>
+      <c r="C64" s="48"/>
       <c r="D64" s="36"/>
       <c r="E64" s="36"/>
       <c r="F64" s="36"/>

</xml_diff>

<commit_message>
V1.0 Fixed some MS Excel releted issue & added pdf to view easily
</commit_message>
<xml_diff>
--- a/Assignment 1.xlsx
+++ b/Assignment 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cffcda41bf3362bc/Software Testing/Test Case Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_D258262CC2B2CBD90605945EC74F8981D2BE7756" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA6BE6B0-FC1A-4379-A00A-72AFD439D3B9}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="11_D258262CC2B2CBD90605945EC74F8981D2BE7756" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E7E0140-6FAC-4FE5-81BA-09ECA0511F83}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,15 @@
     <sheet name="Info" sheetId="1" r:id="rId1"/>
     <sheet name="Create Account" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Create Account'!$A$1:$H$61</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="288">
   <si>
     <t>Project Name</t>
   </si>
@@ -876,6 +879,17 @@
   </si>
   <si>
     <t>password                  123456789</t>
+  </si>
+  <si>
+    <t>Verify providing selected special characters</t>
+  </si>
+  <si>
+    <t>….....
+------
+'''''''''</t>
+  </si>
+  <si>
+    <t>2.9</t>
   </si>
 </sst>
 </file>
@@ -886,7 +900,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -916,11 +930,6 @@
     </font>
     <font>
       <sz val="20"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -977,6 +986,16 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1055,34 +1074,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1091,49 +1110,49 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1142,21 +1161,21 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1166,20 +1185,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1531,7 +1550,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C6" sqref="C6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1"/>
@@ -1599,7 +1618,7 @@
       </c>
       <c r="B6" s="37"/>
       <c r="C6" s="38">
-        <v>45228</v>
+        <v>45230</v>
       </c>
       <c r="D6" s="36"/>
       <c r="E6" s="36"/>
@@ -1619,6 +1638,7 @@
     <mergeCell ref="C4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1628,17 +1648,17 @@
     <tabColor rgb="FFF1C232"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H150"/>
+  <dimension ref="A1:H151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="6.33203125" customWidth="1"/>
     <col min="3" max="3" width="38.21875" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="25.21875" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
     <col min="6" max="6" width="34.6640625" customWidth="1"/>
     <col min="7" max="7" width="14.21875" customWidth="1"/>
@@ -1671,7 +1691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="39.6">
+    <row r="2" spans="1:8" ht="26.4">
       <c r="A2" s="5"/>
       <c r="B2" s="5" t="s">
         <v>17</v>
@@ -1714,10 +1734,10 @@
       <c r="D4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="47"/>
+      <c r="F4" s="48"/>
       <c r="G4" s="46" t="s">
         <v>25</v>
       </c>
@@ -1802,7 +1822,7 @@
       <c r="D9" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="47" t="s">
+      <c r="E9" s="48" t="s">
         <v>43</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -1813,7 +1833,7 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" ht="26.4">
+    <row r="10" spans="1:8" ht="13.2">
       <c r="A10" s="36"/>
       <c r="B10" s="10" t="s">
         <v>46</v>
@@ -1906,7 +1926,7 @@
       <c r="B15" s="8">
         <v>2</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="47" t="s">
         <v>59</v>
       </c>
       <c r="D15" s="36"/>
@@ -2057,21 +2077,21 @@
       </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="1:8" ht="39.6">
+    <row r="22" spans="1:8" ht="52.8">
       <c r="A22" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="34" t="s">
         <v>92</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>93</v>
+        <v>285</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>94</v>
+        <v>286</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>70</v>
@@ -2081,74 +2101,74 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="1:8" ht="15.6">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8">
+    <row r="23" spans="1:8" ht="26.4">
+      <c r="A23" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.6">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8">
         <v>3</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C24" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="9"/>
-    </row>
-    <row r="24" spans="1:8" ht="26.4">
-      <c r="A24" s="8"/>
-      <c r="B24" s="5" t="s">
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" ht="26.4">
+      <c r="A25" s="8"/>
+      <c r="B25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C25" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="24"/>
-    </row>
-    <row r="25" spans="1:8" ht="26.4">
-      <c r="A25" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H25" s="13"/>
-    </row>
-    <row r="26" spans="1:8" ht="39.6">
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="24"/>
+    </row>
+    <row r="26" spans="1:8" ht="26.4">
       <c r="A26" s="8" t="s">
         <v>103</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>106</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D26" s="16"/>
       <c r="E26" s="11" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>25</v>
@@ -2160,22 +2180,22 @@
         <v>109</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>112</v>
+        <v>105</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>106</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="H27" s="13"/>
     </row>
@@ -2184,19 +2204,19 @@
         <v>115</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>45</v>
@@ -2208,190 +2228,188 @@
         <v>121</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="H29" s="13"/>
     </row>
-    <row r="30" spans="1:8" ht="52.8">
+    <row r="30" spans="1:8" ht="39.6">
       <c r="A30" s="8" t="s">
         <v>127</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="26.4">
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31" spans="1:8" ht="52.8">
       <c r="A31" s="8" t="s">
         <v>132</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H31" s="13"/>
-    </row>
-    <row r="32" spans="1:8" ht="52.8">
+    </row>
+    <row r="32" spans="1:8" ht="26.4">
       <c r="A32" s="8" t="s">
         <v>138</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="1:8" ht="39.6">
+    <row r="33" spans="1:8" ht="52.8">
       <c r="A33" s="8" t="s">
         <v>143</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>107</v>
       </c>
       <c r="F33" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="1:8" ht="39.6">
+      <c r="A34" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="G33" s="12" t="s">
+      <c r="G34" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H33" s="13"/>
-    </row>
-    <row r="34" spans="1:8" ht="15.6">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8">
+      <c r="H34" s="13"/>
+    </row>
+    <row r="35" spans="1:8" ht="15.6">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8">
         <v>4</v>
       </c>
-      <c r="C34" s="26" t="s">
+      <c r="C35" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-    </row>
-    <row r="35" spans="1:8" ht="39.6">
-      <c r="A35" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B35" s="5" t="s">
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+    </row>
+    <row r="36" spans="1:8" ht="39.6">
+      <c r="A36" s="8"/>
+      <c r="B36" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C36" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="D35" s="27"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="24"/>
-    </row>
-    <row r="36" spans="1:8" ht="26.4">
-      <c r="A36" s="8" t="s">
+      <c r="D36" s="27"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="24"/>
+    </row>
+    <row r="37" spans="1:8" ht="26.4">
+      <c r="A37" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B37" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C37" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="11" t="s">
+      <c r="D37" s="16"/>
+      <c r="E37" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F37" s="11" t="s">
         <v>155</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H36" s="13"/>
-    </row>
-    <row r="37" spans="1:8" ht="39.6">
-      <c r="A37" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="D37" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>161</v>
       </c>
       <c r="G37" s="12" t="s">
         <v>25</v>
@@ -2400,16 +2418,16 @@
     </row>
     <row r="38" spans="1:8" ht="39.6">
       <c r="A38" s="8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E38" s="16" t="s">
         <v>160</v>
@@ -2424,118 +2442,118 @@
     </row>
     <row r="39" spans="1:8" ht="39.6">
       <c r="A39" s="8" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>169</v>
+        <v>163</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>165</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>171</v>
+        <v>160</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>161</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>25</v>
       </c>
       <c r="H39" s="13"/>
     </row>
-    <row r="40" spans="1:8" ht="26.4">
+    <row r="40" spans="1:8" ht="39.6">
       <c r="A40" s="8" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="D40" s="30" t="s">
-        <v>32</v>
+        <v>168</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>169</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>176</v>
+        <v>170</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>171</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:8" ht="26.4">
       <c r="A41" s="8" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>180</v>
+        <v>174</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>32</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>182</v>
+        <v>175</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>176</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8" ht="26.4">
       <c r="A42" s="8" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>187</v>
+        <v>180</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>181</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G42" s="12" t="s">
         <v>25</v>
       </c>
       <c r="H42" s="13"/>
     </row>
-    <row r="43" spans="1:8" ht="39.6">
+    <row r="43" spans="1:8" ht="26.4">
       <c r="A43" s="8" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>194</v>
+        <v>186</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>188</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>25</v>
@@ -2544,46 +2562,46 @@
     </row>
     <row r="44" spans="1:8" ht="39.6">
       <c r="A44" s="8" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="G44" s="12" t="s">
         <v>25</v>
       </c>
       <c r="H44" s="13"/>
     </row>
-    <row r="45" spans="1:8" ht="26.4">
+    <row r="45" spans="1:8" ht="39.6">
       <c r="A45" s="8" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="D45" s="31" t="s">
-        <v>204</v>
+        <v>197</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>198</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>25</v>
@@ -2592,108 +2610,108 @@
     </row>
     <row r="46" spans="1:8" ht="26.4">
       <c r="A46" s="8" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="D46" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>212</v>
+        <v>203</v>
+      </c>
+      <c r="D46" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>206</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>25</v>
       </c>
       <c r="H46" s="13"/>
     </row>
-    <row r="47" spans="1:8" ht="15.6">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8">
+    <row r="47" spans="1:8" ht="26.4">
+      <c r="A47" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H47" s="13"/>
+    </row>
+    <row r="48" spans="1:8" ht="15.6">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8">
         <v>5</v>
       </c>
-      <c r="C47" s="26" t="s">
+      <c r="C48" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="D47" s="32"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-    </row>
-    <row r="48" spans="1:8" ht="39.6">
-      <c r="A48" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="G48" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H48" s="13" t="s">
-        <v>219</v>
-      </c>
+      <c r="D48" s="32"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8" ht="39.6">
       <c r="A49" s="8" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="E49" s="16" t="s">
-        <v>224</v>
+        <v>215</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11" t="s">
+        <v>217</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G49" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H49" s="13"/>
+      <c r="H49" s="13" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="50" spans="1:8" ht="39.6">
       <c r="A50" s="8" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>228</v>
+        <v>221</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>222</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="E50" s="16" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G50" s="12" t="s">
         <v>25</v>
@@ -2702,22 +2720,22 @@
     </row>
     <row r="51" spans="1:8" ht="39.6">
       <c r="A51" s="8" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>234</v>
+        <v>227</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>228</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G51" s="12" t="s">
         <v>25</v>
@@ -2726,22 +2744,22 @@
     </row>
     <row r="52" spans="1:8" ht="39.6">
       <c r="A52" s="8" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="G52" s="12" t="s">
         <v>25</v>
@@ -2750,43 +2768,43 @@
     </row>
     <row r="53" spans="1:8" ht="39.6">
       <c r="A53" s="8" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="D53" s="33">
-        <v>12345678</v>
+        <v>240</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>241</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="G53" s="12" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="H53" s="13"/>
     </row>
     <row r="54" spans="1:8" ht="39.6">
       <c r="A54" s="8" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>252</v>
+        <v>246</v>
+      </c>
+      <c r="D54" s="33">
+        <v>12345678</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="F54" s="11" t="s">
         <v>248</v>
@@ -2798,19 +2816,19 @@
     </row>
     <row r="55" spans="1:8" ht="39.6">
       <c r="A55" s="8" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="F55" s="11" t="s">
         <v>248</v>
@@ -2822,19 +2840,19 @@
     </row>
     <row r="56" spans="1:8" ht="39.6">
       <c r="A56" s="8" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="D56" s="14" t="s">
-        <v>284</v>
+        <v>256</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>257</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>248</v>
@@ -2846,19 +2864,19 @@
     </row>
     <row r="57" spans="1:8" ht="39.6">
       <c r="A57" s="8" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>266</v>
+        <v>261</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>284</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F57" s="11" t="s">
         <v>248</v>
@@ -2868,21 +2886,21 @@
       </c>
       <c r="H57" s="13"/>
     </row>
-    <row r="58" spans="1:8" ht="26.4">
+    <row r="58" spans="1:8" ht="39.6">
       <c r="A58" s="8" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>270</v>
+        <v>264</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>265</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F58" s="11" t="s">
         <v>248</v>
@@ -2894,19 +2912,19 @@
     </row>
     <row r="59" spans="1:8" ht="26.4">
       <c r="A59" s="8" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="F59" s="11" t="s">
         <v>248</v>
@@ -2918,47 +2936,61 @@
     </row>
     <row r="60" spans="1:8" ht="26.4">
       <c r="A60" s="8" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>283</v>
+        <v>275</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>276</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>282</v>
+        <v>248</v>
       </c>
       <c r="G60" s="12" t="s">
         <v>45</v>
       </c>
       <c r="H60" s="13"/>
     </row>
-    <row r="61" spans="1:8" ht="15.6" hidden="1">
-      <c r="A61" s="8"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="48"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="9"/>
+    <row r="61" spans="1:8" ht="26.4">
+      <c r="A61" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="G61" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:8" ht="15.6" hidden="1">
       <c r="A62" s="8"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="13"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="36"/>
+      <c r="G62" s="36"/>
+      <c r="H62" s="9"/>
     </row>
     <row r="63" spans="1:8" ht="15.6" hidden="1">
       <c r="A63" s="8"/>
@@ -2972,23 +3004,23 @@
     </row>
     <row r="64" spans="1:8" ht="15.6" hidden="1">
       <c r="A64" s="8"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="48"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="36"/>
-      <c r="H64" s="9"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:8" ht="15.6" hidden="1">
       <c r="A65" s="8"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="13"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="44"/>
+      <c r="D65" s="36"/>
+      <c r="E65" s="36"/>
+      <c r="F65" s="36"/>
+      <c r="G65" s="36"/>
+      <c r="H65" s="9"/>
     </row>
     <row r="66" spans="1:8" ht="15.6" hidden="1">
       <c r="A66" s="8"/>
@@ -3002,36 +3034,36 @@
     </row>
     <row r="67" spans="1:8" ht="15.6" hidden="1">
       <c r="A67" s="8"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="13"/>
     </row>
     <row r="68" spans="1:8" ht="15.6" hidden="1">
       <c r="A68" s="8"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="13"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
     </row>
     <row r="69" spans="1:8" ht="15.6" hidden="1">
       <c r="A69" s="8"/>
       <c r="B69" s="10"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
       <c r="G69" s="12"/>
       <c r="H69" s="13"/>
     </row>
-    <row r="70" spans="1:8" ht="13.2">
-      <c r="A70" s="10"/>
+    <row r="70" spans="1:8" ht="15.6" hidden="1">
+      <c r="A70" s="8"/>
       <c r="B70" s="10"/>
       <c r="C70" s="14"/>
       <c r="D70" s="14"/>
@@ -3040,830 +3072,103 @@
       <c r="G70" s="12"/>
       <c r="H70" s="13"/>
     </row>
-    <row r="71" spans="1:8" ht="13.2">
-      <c r="A71" s="10"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="13"/>
-    </row>
-    <row r="72" spans="1:8" ht="13.2">
-      <c r="A72" s="10"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="13"/>
-    </row>
-    <row r="73" spans="1:8" ht="13.2">
-      <c r="A73" s="10"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="12"/>
-      <c r="H73" s="13"/>
-    </row>
-    <row r="74" spans="1:8" ht="13.2">
-      <c r="A74" s="10"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="12"/>
-      <c r="H74" s="13"/>
-    </row>
-    <row r="75" spans="1:8" ht="13.2">
-      <c r="A75" s="10"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="13"/>
-    </row>
-    <row r="76" spans="1:8" ht="15.6" hidden="1">
-      <c r="A76" s="8"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="44"/>
-      <c r="D76" s="36"/>
-      <c r="E76" s="36"/>
-      <c r="F76" s="36"/>
-      <c r="G76" s="36"/>
-      <c r="H76" s="9"/>
-    </row>
-    <row r="77" spans="1:8" ht="13.2">
-      <c r="A77" s="10"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="13"/>
-    </row>
-    <row r="78" spans="1:8" ht="13.2">
-      <c r="A78" s="10"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="14"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="13"/>
-    </row>
-    <row r="79" spans="1:8" ht="13.2">
-      <c r="A79" s="10"/>
-      <c r="B79" s="10"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="14"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="13"/>
-    </row>
-    <row r="80" spans="1:8" ht="13.2">
-      <c r="A80" s="10"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="13"/>
-    </row>
-    <row r="81" spans="1:8" ht="13.2">
-      <c r="A81" s="10"/>
-      <c r="B81" s="10"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="13"/>
-    </row>
-    <row r="82" spans="1:8" ht="13.2">
-      <c r="A82" s="10"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="14"/>
-      <c r="D82" s="14"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="12"/>
-      <c r="H82" s="13"/>
-    </row>
-    <row r="83" spans="1:8" ht="13.2">
-      <c r="A83" s="10"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="13"/>
-    </row>
-    <row r="84" spans="1:8" ht="15.6">
-      <c r="A84" s="8"/>
-      <c r="B84" s="8"/>
-      <c r="C84" s="44"/>
-      <c r="D84" s="36"/>
-      <c r="E84" s="36"/>
-      <c r="F84" s="36"/>
-      <c r="G84" s="36"/>
-      <c r="H84" s="9"/>
-    </row>
-    <row r="85" spans="1:8" ht="13.2">
-      <c r="A85" s="10"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
-      <c r="E85" s="11"/>
-      <c r="F85" s="11"/>
-      <c r="G85" s="12"/>
-      <c r="H85" s="13"/>
-    </row>
-    <row r="86" spans="1:8" ht="13.2">
-      <c r="A86" s="10"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="14"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
-      <c r="G86" s="12"/>
-      <c r="H86" s="13"/>
-    </row>
-    <row r="87" spans="1:8" ht="13.2">
-      <c r="A87" s="10"/>
-      <c r="B87" s="10"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="12"/>
-      <c r="H87" s="13"/>
-    </row>
-    <row r="88" spans="1:8" ht="13.2">
-      <c r="A88" s="10"/>
-      <c r="B88" s="10"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="11"/>
-      <c r="F88" s="11"/>
-      <c r="G88" s="12"/>
-      <c r="H88" s="13"/>
-    </row>
-    <row r="89" spans="1:8" ht="15.6">
-      <c r="A89" s="8"/>
-      <c r="B89" s="8"/>
-      <c r="C89" s="44"/>
-      <c r="D89" s="36"/>
-      <c r="E89" s="36"/>
-      <c r="F89" s="36"/>
-      <c r="G89" s="36"/>
-      <c r="H89" s="9"/>
-    </row>
-    <row r="90" spans="1:8" ht="13.2">
-      <c r="A90" s="10"/>
-      <c r="B90" s="10"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
-      <c r="F90" s="11"/>
-      <c r="G90" s="12"/>
-      <c r="H90" s="13"/>
-    </row>
-    <row r="91" spans="1:8" ht="13.2">
-      <c r="A91" s="10"/>
-      <c r="B91" s="10"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
-      <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
-      <c r="G91" s="12"/>
-      <c r="H91" s="13"/>
-    </row>
-    <row r="92" spans="1:8" ht="13.2">
-      <c r="A92" s="10"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="11"/>
-      <c r="F92" s="11"/>
-      <c r="G92" s="12"/>
-      <c r="H92" s="13"/>
-    </row>
-    <row r="93" spans="1:8" ht="13.2">
-      <c r="A93" s="10"/>
-      <c r="B93" s="10"/>
-      <c r="C93" s="14"/>
-      <c r="D93" s="14"/>
-      <c r="E93" s="14"/>
-      <c r="F93" s="14"/>
-      <c r="G93" s="12"/>
-      <c r="H93" s="13"/>
-    </row>
-    <row r="94" spans="1:8" ht="13.2">
-      <c r="A94" s="10"/>
-      <c r="B94" s="10"/>
-      <c r="C94" s="14"/>
-      <c r="D94" s="14"/>
-      <c r="E94" s="11"/>
-      <c r="F94" s="11"/>
-      <c r="G94" s="12"/>
-      <c r="H94" s="13"/>
-    </row>
-    <row r="95" spans="1:8" ht="15.6">
-      <c r="A95" s="8"/>
-      <c r="B95" s="8"/>
-      <c r="C95" s="44"/>
-      <c r="D95" s="36"/>
-      <c r="E95" s="36"/>
-      <c r="F95" s="36"/>
-      <c r="G95" s="36"/>
-      <c r="H95" s="9"/>
-    </row>
-    <row r="96" spans="1:8" ht="13.2">
-      <c r="A96" s="10"/>
-      <c r="B96" s="10"/>
-      <c r="C96" s="11"/>
-      <c r="D96" s="11"/>
-      <c r="E96" s="11"/>
-      <c r="F96" s="11"/>
-      <c r="G96" s="12"/>
-      <c r="H96" s="13"/>
-    </row>
-    <row r="97" spans="1:8" ht="13.2">
-      <c r="A97" s="10"/>
-      <c r="B97" s="10"/>
-      <c r="C97" s="14"/>
-      <c r="D97" s="14"/>
-      <c r="E97" s="11"/>
-      <c r="F97" s="11"/>
-      <c r="G97" s="12"/>
-      <c r="H97" s="13"/>
-    </row>
-    <row r="98" spans="1:8" ht="13.2">
-      <c r="A98" s="10"/>
-      <c r="B98" s="10"/>
-      <c r="C98" s="14"/>
-      <c r="D98" s="14"/>
-      <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
-      <c r="G98" s="12"/>
-      <c r="H98" s="13"/>
-    </row>
-    <row r="99" spans="1:8" ht="13.2">
-      <c r="A99" s="10"/>
-      <c r="B99" s="10"/>
-      <c r="C99" s="14"/>
-      <c r="D99" s="14"/>
-      <c r="E99" s="14"/>
-      <c r="F99" s="14"/>
-      <c r="G99" s="12"/>
-      <c r="H99" s="13"/>
-    </row>
-    <row r="100" spans="1:8" ht="13.2">
-      <c r="A100" s="10"/>
-      <c r="B100" s="10"/>
-      <c r="C100" s="14"/>
-      <c r="D100" s="14"/>
-      <c r="E100" s="11"/>
-      <c r="F100" s="11"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="13"/>
-    </row>
-    <row r="101" spans="1:8" ht="15.6">
-      <c r="A101" s="8"/>
-      <c r="B101" s="8"/>
-      <c r="C101" s="44"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="36"/>
-      <c r="F101" s="36"/>
-      <c r="G101" s="36"/>
-      <c r="H101" s="9"/>
-    </row>
-    <row r="102" spans="1:8" ht="13.2">
-      <c r="A102" s="10"/>
-      <c r="B102" s="10"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
-      <c r="F102" s="11"/>
-      <c r="G102" s="12"/>
-      <c r="H102" s="13"/>
-    </row>
-    <row r="103" spans="1:8" ht="13.2">
-      <c r="A103" s="10"/>
-      <c r="B103" s="10"/>
-      <c r="C103" s="14"/>
-      <c r="D103" s="14"/>
-      <c r="E103" s="11"/>
-      <c r="F103" s="11"/>
-      <c r="G103" s="12"/>
-      <c r="H103" s="13"/>
-    </row>
-    <row r="104" spans="1:8" ht="13.2">
-      <c r="A104" s="10"/>
-      <c r="B104" s="10"/>
-      <c r="C104" s="14"/>
-      <c r="D104" s="14"/>
-      <c r="E104" s="11"/>
-      <c r="F104" s="11"/>
-      <c r="G104" s="12"/>
-      <c r="H104" s="13"/>
-    </row>
-    <row r="105" spans="1:8" ht="13.2">
-      <c r="A105" s="10"/>
-      <c r="B105" s="10"/>
-      <c r="C105" s="14"/>
-      <c r="D105" s="14"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="14"/>
-      <c r="G105" s="12"/>
-      <c r="H105" s="13"/>
-    </row>
-    <row r="106" spans="1:8" ht="13.2">
-      <c r="A106" s="10"/>
-      <c r="B106" s="10"/>
-      <c r="C106" s="14"/>
-      <c r="D106" s="14"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="14"/>
-      <c r="G106" s="12"/>
-      <c r="H106" s="13"/>
-    </row>
-    <row r="107" spans="1:8" ht="13.2">
-      <c r="A107" s="10"/>
-      <c r="B107" s="10"/>
-      <c r="C107" s="14"/>
-      <c r="D107" s="14"/>
-      <c r="E107" s="14"/>
-      <c r="F107" s="14"/>
-      <c r="G107" s="12"/>
-      <c r="H107" s="13"/>
-    </row>
-    <row r="108" spans="1:8" ht="13.2">
-      <c r="A108" s="10"/>
-      <c r="B108" s="10"/>
-      <c r="C108" s="14"/>
-      <c r="D108" s="14"/>
-      <c r="E108" s="14"/>
-      <c r="F108" s="14"/>
-      <c r="G108" s="12"/>
-      <c r="H108" s="13"/>
-    </row>
-    <row r="109" spans="1:8" ht="13.2">
-      <c r="A109" s="10"/>
-      <c r="B109" s="10"/>
-      <c r="C109" s="14"/>
-      <c r="D109" s="14"/>
-      <c r="E109" s="14"/>
-      <c r="F109" s="14"/>
-      <c r="G109" s="12"/>
-      <c r="H109" s="13"/>
-    </row>
-    <row r="110" spans="1:8" ht="13.2">
-      <c r="A110" s="10"/>
-      <c r="B110" s="10"/>
-      <c r="C110" s="14"/>
-      <c r="D110" s="14"/>
-      <c r="E110" s="14"/>
-      <c r="F110" s="14"/>
-      <c r="G110" s="12"/>
-      <c r="H110" s="13"/>
-    </row>
-    <row r="111" spans="1:8" ht="15.6">
-      <c r="A111" s="8"/>
-      <c r="B111" s="8"/>
-      <c r="C111" s="44"/>
-      <c r="D111" s="36"/>
-      <c r="E111" s="36"/>
-      <c r="F111" s="36"/>
-      <c r="G111" s="36"/>
-      <c r="H111" s="9"/>
-    </row>
-    <row r="112" spans="1:8" ht="13.2">
-      <c r="A112" s="10"/>
-      <c r="B112" s="10"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
-      <c r="E112" s="11"/>
-      <c r="F112" s="11"/>
-      <c r="G112" s="12"/>
-      <c r="H112" s="13"/>
-    </row>
-    <row r="113" spans="1:8" ht="13.2">
-      <c r="A113" s="10"/>
-      <c r="B113" s="10"/>
-      <c r="C113" s="14"/>
-      <c r="D113" s="14"/>
-      <c r="E113" s="11"/>
-      <c r="F113" s="11"/>
-      <c r="G113" s="12"/>
-      <c r="H113" s="13"/>
-    </row>
-    <row r="114" spans="1:8" ht="13.2">
-      <c r="A114" s="10"/>
-      <c r="B114" s="10"/>
-      <c r="C114" s="14"/>
-      <c r="D114" s="14"/>
-      <c r="E114" s="11"/>
-      <c r="F114" s="11"/>
-      <c r="G114" s="12"/>
-      <c r="H114" s="13"/>
-    </row>
-    <row r="115" spans="1:8" ht="13.2">
-      <c r="A115" s="10"/>
-      <c r="B115" s="10"/>
-      <c r="C115" s="14"/>
-      <c r="D115" s="14"/>
-      <c r="E115" s="14"/>
-      <c r="F115" s="14"/>
-      <c r="G115" s="12"/>
-      <c r="H115" s="13"/>
-    </row>
-    <row r="116" spans="1:8" ht="13.2">
-      <c r="A116" s="10"/>
-      <c r="B116" s="10"/>
-      <c r="C116" s="14"/>
-      <c r="D116" s="14"/>
-      <c r="E116" s="14"/>
-      <c r="F116" s="14"/>
-      <c r="G116" s="12"/>
-      <c r="H116" s="13"/>
-    </row>
-    <row r="117" spans="1:8" ht="13.2">
-      <c r="A117" s="10"/>
-      <c r="B117" s="10"/>
-      <c r="C117" s="14"/>
-      <c r="D117" s="14"/>
-      <c r="E117" s="14"/>
-      <c r="F117" s="14"/>
-      <c r="G117" s="12"/>
-      <c r="H117" s="13"/>
-    </row>
-    <row r="118" spans="1:8" ht="13.2">
-      <c r="A118" s="10"/>
-      <c r="B118" s="10"/>
-      <c r="C118" s="14"/>
-      <c r="D118" s="14"/>
-      <c r="E118" s="14"/>
-      <c r="F118" s="14"/>
-      <c r="G118" s="12"/>
-      <c r="H118" s="13"/>
-    </row>
-    <row r="119" spans="1:8" ht="13.2">
-      <c r="A119" s="10"/>
-      <c r="B119" s="10"/>
-      <c r="C119" s="14"/>
-      <c r="D119" s="14"/>
-      <c r="E119" s="14"/>
-      <c r="F119" s="14"/>
-      <c r="G119" s="12"/>
-      <c r="H119" s="13"/>
-    </row>
-    <row r="120" spans="1:8" ht="13.2">
-      <c r="A120" s="10"/>
-      <c r="B120" s="10"/>
-      <c r="C120" s="14"/>
-      <c r="D120" s="14"/>
-      <c r="E120" s="14"/>
-      <c r="F120" s="14"/>
-      <c r="G120" s="12"/>
-      <c r="H120" s="13"/>
-    </row>
-    <row r="121" spans="1:8" ht="13.2">
-      <c r="A121" s="10"/>
-      <c r="B121" s="10"/>
-      <c r="C121" s="14"/>
-      <c r="D121" s="14"/>
-      <c r="E121" s="14"/>
-      <c r="F121" s="14"/>
-      <c r="G121" s="12"/>
-      <c r="H121" s="13"/>
-    </row>
-    <row r="122" spans="1:8" ht="15.6">
-      <c r="A122" s="8"/>
-      <c r="B122" s="8"/>
-      <c r="C122" s="44"/>
-      <c r="D122" s="36"/>
-      <c r="E122" s="36"/>
-      <c r="F122" s="36"/>
-      <c r="G122" s="36"/>
-      <c r="H122" s="9"/>
-    </row>
-    <row r="123" spans="1:8" ht="13.2">
-      <c r="A123" s="10"/>
-      <c r="B123" s="10"/>
-      <c r="C123" s="11"/>
-      <c r="D123" s="11"/>
-      <c r="E123" s="11"/>
-      <c r="F123" s="11"/>
-      <c r="G123" s="12"/>
-      <c r="H123" s="13"/>
-    </row>
-    <row r="124" spans="1:8" ht="13.2">
-      <c r="A124" s="10"/>
-      <c r="B124" s="10"/>
-      <c r="C124" s="14"/>
-      <c r="D124" s="14"/>
-      <c r="E124" s="14"/>
-      <c r="F124" s="14"/>
-      <c r="G124" s="12"/>
-      <c r="H124" s="13"/>
-    </row>
-    <row r="125" spans="1:8" ht="13.2">
-      <c r="A125" s="10"/>
-      <c r="B125" s="10"/>
-      <c r="C125" s="14"/>
-      <c r="D125" s="14"/>
-      <c r="E125" s="14"/>
-      <c r="F125" s="14"/>
-      <c r="G125" s="12"/>
-      <c r="H125" s="13"/>
-    </row>
-    <row r="126" spans="1:8" ht="13.2">
-      <c r="A126" s="10"/>
-      <c r="B126" s="10"/>
-      <c r="C126" s="14"/>
-      <c r="D126" s="14"/>
-      <c r="E126" s="14"/>
-      <c r="F126" s="14"/>
-      <c r="G126" s="12"/>
-      <c r="H126" s="13"/>
-    </row>
-    <row r="127" spans="1:8" ht="13.2">
-      <c r="A127" s="10"/>
-      <c r="B127" s="10"/>
-      <c r="C127" s="14"/>
-      <c r="D127" s="14"/>
-      <c r="E127" s="14"/>
-      <c r="F127" s="14"/>
-      <c r="G127" s="12"/>
-      <c r="H127" s="13"/>
-    </row>
-    <row r="128" spans="1:8" ht="13.2">
-      <c r="A128" s="10"/>
-      <c r="B128" s="10"/>
-      <c r="C128" s="14"/>
-      <c r="D128" s="14"/>
-      <c r="E128" s="14"/>
-      <c r="F128" s="14"/>
-      <c r="G128" s="12"/>
-      <c r="H128" s="13"/>
-    </row>
-    <row r="129" spans="1:8" ht="15.6">
-      <c r="A129" s="8"/>
-      <c r="B129" s="8"/>
-      <c r="C129" s="44"/>
-      <c r="D129" s="36"/>
-      <c r="E129" s="36"/>
-      <c r="F129" s="36"/>
-      <c r="G129" s="36"/>
-      <c r="H129" s="9"/>
-    </row>
-    <row r="130" spans="1:8" ht="13.2">
-      <c r="A130" s="10"/>
-      <c r="B130" s="10"/>
-      <c r="C130" s="16"/>
-      <c r="D130" s="16"/>
-      <c r="E130" s="11"/>
-      <c r="F130" s="11"/>
-      <c r="G130" s="12"/>
-      <c r="H130" s="13"/>
-    </row>
-    <row r="131" spans="1:8" ht="13.2">
-      <c r="A131" s="10"/>
-      <c r="B131" s="10"/>
-      <c r="C131" s="16"/>
-      <c r="D131" s="16"/>
-      <c r="E131" s="11"/>
-      <c r="F131" s="11"/>
-      <c r="G131" s="12"/>
-      <c r="H131" s="13"/>
-    </row>
-    <row r="132" spans="1:8" ht="13.2">
-      <c r="A132" s="10"/>
-      <c r="B132" s="10"/>
-      <c r="C132" s="16"/>
-      <c r="D132" s="16"/>
-      <c r="E132" s="11"/>
-      <c r="F132" s="11"/>
-      <c r="G132" s="12"/>
-      <c r="H132" s="13"/>
-    </row>
-    <row r="133" spans="1:8" ht="15.6">
-      <c r="A133" s="8"/>
-      <c r="B133" s="8"/>
-      <c r="C133" s="44"/>
-      <c r="D133" s="36"/>
-      <c r="E133" s="36"/>
-      <c r="F133" s="36"/>
-      <c r="G133" s="36"/>
-      <c r="H133" s="32"/>
-    </row>
-    <row r="134" spans="1:8" ht="13.2">
-      <c r="A134" s="10"/>
-      <c r="B134" s="10"/>
-      <c r="C134" s="11"/>
-      <c r="D134" s="11"/>
-      <c r="E134" s="11"/>
-      <c r="F134" s="11"/>
-      <c r="G134" s="12"/>
-      <c r="H134" s="34"/>
-    </row>
-    <row r="135" spans="1:8" ht="13.2">
-      <c r="A135" s="10"/>
-      <c r="B135" s="10"/>
-      <c r="C135" s="14"/>
-      <c r="D135" s="14"/>
-      <c r="E135" s="14"/>
-      <c r="F135" s="14"/>
-      <c r="G135" s="12"/>
-      <c r="H135" s="34"/>
-    </row>
-    <row r="136" spans="1:8" ht="13.2">
-      <c r="A136" s="10"/>
-      <c r="B136" s="10"/>
-      <c r="C136" s="14"/>
-      <c r="D136" s="14"/>
-      <c r="E136" s="14"/>
-      <c r="F136" s="14"/>
-      <c r="G136" s="12"/>
-      <c r="H136" s="34"/>
-    </row>
-    <row r="137" spans="1:8" ht="13.2">
-      <c r="A137" s="10"/>
-      <c r="B137" s="10"/>
-      <c r="C137" s="14"/>
-      <c r="D137" s="14"/>
-      <c r="E137" s="14"/>
-      <c r="F137" s="14"/>
-      <c r="G137" s="12"/>
-      <c r="H137" s="34"/>
-    </row>
-    <row r="138" spans="1:8" ht="13.2">
-      <c r="A138" s="10"/>
-      <c r="B138" s="10"/>
-      <c r="C138" s="14"/>
-      <c r="D138" s="14"/>
-      <c r="E138" s="11"/>
-      <c r="F138" s="11"/>
-      <c r="G138" s="12"/>
-      <c r="H138" s="34"/>
-    </row>
-    <row r="139" spans="1:8" ht="13.2">
-      <c r="A139" s="10"/>
-      <c r="B139" s="10"/>
-      <c r="C139" s="14"/>
-      <c r="D139" s="14"/>
-      <c r="E139" s="14"/>
-      <c r="F139" s="14"/>
-      <c r="G139" s="12"/>
-      <c r="H139" s="34"/>
-    </row>
-    <row r="140" spans="1:8" ht="13.2">
-      <c r="A140" s="10"/>
-      <c r="B140" s="10"/>
-      <c r="C140" s="14"/>
-      <c r="D140" s="14"/>
-      <c r="E140" s="14"/>
-      <c r="F140" s="14"/>
-      <c r="G140" s="12"/>
-      <c r="H140" s="34"/>
-    </row>
-    <row r="141" spans="1:8" ht="13.2">
-      <c r="A141" s="10"/>
-      <c r="B141" s="10"/>
-      <c r="C141" s="14"/>
-      <c r="D141" s="14"/>
-      <c r="E141" s="14"/>
-      <c r="F141" s="14"/>
-      <c r="G141" s="12"/>
-      <c r="H141" s="34"/>
-    </row>
-    <row r="142" spans="1:8" ht="13.2">
-      <c r="A142" s="10"/>
-      <c r="B142" s="10"/>
-      <c r="C142" s="14"/>
-      <c r="D142" s="14"/>
-      <c r="E142" s="11"/>
-      <c r="F142" s="11"/>
-      <c r="G142" s="12"/>
-      <c r="H142" s="34"/>
-    </row>
-    <row r="143" spans="1:8" ht="13.2">
-      <c r="A143" s="10"/>
-      <c r="B143" s="10"/>
-      <c r="C143" s="14"/>
-      <c r="D143" s="14"/>
-      <c r="E143" s="14"/>
-      <c r="F143" s="14"/>
-      <c r="G143" s="12"/>
-      <c r="H143" s="34"/>
-    </row>
-    <row r="144" spans="1:8" ht="13.2">
-      <c r="A144" s="10"/>
-      <c r="B144" s="10"/>
-      <c r="C144" s="14"/>
-      <c r="D144" s="14"/>
-      <c r="E144" s="14"/>
-      <c r="F144" s="14"/>
-      <c r="G144" s="12"/>
-      <c r="H144" s="34"/>
-    </row>
-    <row r="145" spans="1:8" ht="13.2">
-      <c r="A145" s="10"/>
-      <c r="B145" s="10"/>
-      <c r="C145" s="14"/>
-      <c r="D145" s="14"/>
-      <c r="E145" s="14"/>
-      <c r="F145" s="14"/>
-      <c r="G145" s="12"/>
-      <c r="H145" s="34"/>
-    </row>
-    <row r="146" spans="1:8" ht="13.2">
-      <c r="A146" s="10"/>
-      <c r="B146" s="10"/>
-      <c r="C146" s="14"/>
-      <c r="D146" s="14"/>
-      <c r="E146" s="14"/>
-      <c r="F146" s="14"/>
-      <c r="G146" s="12"/>
-      <c r="H146" s="34"/>
-    </row>
-    <row r="147" spans="1:8" ht="13.2">
-      <c r="A147" s="10"/>
-      <c r="B147" s="10"/>
-      <c r="C147" s="14"/>
-      <c r="D147" s="14"/>
-      <c r="E147" s="14"/>
-      <c r="F147" s="14"/>
-      <c r="G147" s="12"/>
-      <c r="H147" s="34"/>
-    </row>
-    <row r="148" spans="1:8" ht="13.2">
-      <c r="A148" s="10"/>
-      <c r="B148" s="10"/>
-      <c r="C148" s="14"/>
-      <c r="D148" s="14"/>
-      <c r="E148" s="14"/>
-      <c r="F148" s="14"/>
-      <c r="G148" s="12"/>
-      <c r="H148" s="34"/>
-    </row>
-    <row r="149" spans="1:8" ht="13.2">
-      <c r="A149" s="10"/>
-      <c r="B149" s="10"/>
-      <c r="C149" s="14"/>
-      <c r="D149" s="14"/>
-      <c r="E149" s="14"/>
-      <c r="F149" s="14"/>
-      <c r="G149" s="12"/>
-      <c r="H149" s="34"/>
-    </row>
-    <row r="150" spans="1:8" ht="13.2">
-      <c r="A150" s="10"/>
-      <c r="B150" s="10"/>
-      <c r="C150" s="14"/>
-      <c r="D150" s="14"/>
-      <c r="E150" s="14"/>
-      <c r="F150" s="14"/>
-      <c r="G150" s="12"/>
-      <c r="H150" s="34"/>
-    </row>
+    <row r="71" spans="1:8" ht="13.2"/>
+    <row r="72" spans="1:8" ht="13.2"/>
+    <row r="73" spans="1:8" ht="13.2"/>
+    <row r="74" spans="1:8" ht="13.2"/>
+    <row r="75" spans="1:8" ht="13.2"/>
+    <row r="76" spans="1:8" ht="13.2"/>
+    <row r="77" spans="1:8" ht="13.2" hidden="1"/>
+    <row r="78" spans="1:8" ht="13.2"/>
+    <row r="79" spans="1:8" ht="13.2"/>
+    <row r="80" spans="1:8" ht="13.2"/>
+    <row r="81" ht="13.2"/>
+    <row r="82" ht="13.2"/>
+    <row r="83" ht="13.2"/>
+    <row r="84" ht="13.2"/>
+    <row r="85" ht="13.2"/>
+    <row r="86" ht="13.2"/>
+    <row r="87" ht="13.2"/>
+    <row r="88" ht="13.2"/>
+    <row r="89" ht="13.2"/>
+    <row r="90" ht="13.2"/>
+    <row r="91" ht="13.2"/>
+    <row r="92" ht="13.2"/>
+    <row r="93" ht="13.2"/>
+    <row r="94" ht="13.2"/>
+    <row r="95" ht="13.2"/>
+    <row r="96" ht="13.2"/>
+    <row r="97" ht="13.2"/>
+    <row r="98" ht="13.2"/>
+    <row r="99" ht="13.2"/>
+    <row r="100" ht="13.2"/>
+    <row r="101" ht="13.2"/>
+    <row r="102" ht="13.2"/>
+    <row r="103" ht="13.2"/>
+    <row r="104" ht="13.2"/>
+    <row r="105" ht="13.2"/>
+    <row r="106" ht="13.2"/>
+    <row r="107" ht="13.2"/>
+    <row r="108" ht="13.2"/>
+    <row r="109" ht="13.2"/>
+    <row r="110" ht="13.2"/>
+    <row r="111" ht="13.2"/>
+    <row r="112" ht="13.2"/>
+    <row r="113" ht="13.2"/>
+    <row r="114" ht="13.2"/>
+    <row r="115" ht="13.2"/>
+    <row r="116" ht="13.2"/>
+    <row r="117" ht="13.2"/>
+    <row r="118" ht="13.2"/>
+    <row r="119" ht="13.2"/>
+    <row r="120" ht="13.2"/>
+    <row r="121" ht="13.2"/>
+    <row r="122" ht="13.2"/>
+    <row r="123" ht="13.2"/>
+    <row r="124" ht="13.2"/>
+    <row r="125" ht="13.2"/>
+    <row r="126" ht="13.2"/>
+    <row r="127" ht="13.2"/>
+    <row r="128" ht="13.2"/>
+    <row r="129" ht="13.2"/>
+    <row r="130" ht="13.2"/>
+    <row r="131" ht="13.2"/>
+    <row r="132" ht="13.2"/>
+    <row r="133" ht="13.2"/>
+    <row r="134" ht="13.2"/>
+    <row r="135" ht="13.2"/>
+    <row r="136" ht="13.2"/>
+    <row r="137" ht="13.2"/>
+    <row r="138" ht="13.2"/>
+    <row r="139" ht="13.2"/>
+    <row r="140" ht="13.2"/>
+    <row r="141" ht="13.2"/>
+    <row r="142" ht="13.2"/>
+    <row r="143" ht="13.2"/>
+    <row r="144" ht="13.2"/>
+    <row r="145" ht="13.2"/>
+    <row r="146" ht="13.2"/>
+    <row r="147" ht="13.2"/>
+    <row r="148" ht="13.2"/>
+    <row r="149" ht="13.2"/>
+    <row r="150" ht="13.2"/>
+    <row r="151" ht="13.2"/>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="11">
+    <mergeCell ref="C62:G62"/>
+    <mergeCell ref="C65:G65"/>
     <mergeCell ref="A4:A8"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="G9:G13"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
     <mergeCell ref="E4:E8"/>
     <mergeCell ref="F4:F8"/>
     <mergeCell ref="G4:G8"/>
     <mergeCell ref="E9:E13"/>
     <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C61:G61"/>
-    <mergeCell ref="C64:G64"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="C84:G84"/>
-    <mergeCell ref="C89:G89"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="C122:G122"/>
-    <mergeCell ref="C129:G129"/>
-    <mergeCell ref="C133:G133"/>
   </mergeCells>
-  <conditionalFormatting sqref="G4:G14 G16:G22 G24:G33 G35:G46 G48:G60 G62:G63 G65:G66 G68:G75 G77:G83 G85:G88 G90:G94 G96:G100 G102:G110 G112:G121 G123:G128 G130:G132 G134:G150">
+  <phoneticPr fontId="17" type="noConversion"/>
+  <conditionalFormatting sqref="G4:G14 G16:G23 G25:G34 G36:G47 G49:G61 G63:G64 G66:G67 G69:G70">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(G4))))</formula>
     </cfRule>
@@ -3875,13 +3180,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4 G9 G14 G16:G22 G24:G33 G35:G46 G48:G60 G62:G63 G65:G66 G68:G75 G77:G83 G85:G88 G90:G94 G96:G100 G102:G110 G112:G121 G123:G128 G130:G132 G134:G150" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4 G9 G14 G16:G23 G25:G34 G36:G47 G49:G61 G63:G64 G66:G67 G69:G70" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Ready to Test,Pass,Fail,Block / Skip"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" scale="95" orientation="landscape" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
V1.1 1 test case fixed (TC11)
</commit_message>
<xml_diff>
--- a/Assignment 1.xlsx
+++ b/Assignment 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cffcda41bf3362bc/Software Testing/Test Case Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_D258262CC2B2CBD90605945EC74F8981D2BE7756" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E7E0140-6FAC-4FE5-81BA-09ECA0511F83}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="11_D258262CC2B2CBD90605945EC74F8981D2BE7756" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8528745C-5845-4459-A2BC-2FA60FF11DC6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="289">
   <si>
     <t>Project Name</t>
   </si>
@@ -303,15 +303,6 @@
   </si>
   <si>
     <t>2.8</t>
-  </si>
-  <si>
-    <t>Verify if the name accepts more than 42 English characters</t>
-  </si>
-  <si>
-    <t>absdehgafsabsdehgafsabsdehgafsabsdehgafsabsdehgafs</t>
-  </si>
-  <si>
-    <t>An error should appear saying, "The name should not be more than 42 characters."</t>
   </si>
   <si>
     <t>Create account using invalid "Email"</t>
@@ -890,6 +881,18 @@
   </si>
   <si>
     <t>2.9</t>
+  </si>
+  <si>
+    <t>Verify if the name accepts more than 100 English characters</t>
+  </si>
+  <si>
+    <t>ghftywsdfgghftywsdfgghftywsdfgghftywsdfgghftywsdfgghftywsdfgghftywsdfgghftywsdfgghftywsdfgghftywsdfg4</t>
+  </si>
+  <si>
+    <t>An error should appear saying, "The name should not be more than 100 characters."</t>
+  </si>
+  <si>
+    <t>An error appeared that "Name maximum 100 characters."</t>
   </si>
 </sst>
 </file>
@@ -900,7 +903,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -997,6 +1000,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1066,7 +1080,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1198,6 +1212,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1549,7 +1569,7 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6:E6"/>
     </sheetView>
   </sheetViews>
@@ -1650,8 +1670,8 @@
   </sheetPr>
   <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2085,10 +2105,10 @@
         <v>92</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>90</v>
@@ -2101,27 +2121,27 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="1:8" ht="26.4">
+    <row r="23" spans="1:8" ht="52.8">
       <c r="A23" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B23" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>285</v>
+      </c>
+      <c r="D23" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="E23" s="50" t="s">
         <v>287</v>
       </c>
-      <c r="C23" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>70</v>
+      <c r="F23" s="50" t="s">
+        <v>288</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="H23" s="13"/>
     </row>
@@ -2131,7 +2151,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="47" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D24" s="36"/>
       <c r="E24" s="36"/>
@@ -2145,7 +2165,7 @@
         <v>17</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="22"/>
@@ -2155,20 +2175,20 @@
     </row>
     <row r="26" spans="1:8" ht="26.4">
       <c r="A26" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>25</v>
@@ -2177,22 +2197,22 @@
     </row>
     <row r="27" spans="1:8" ht="39.6">
       <c r="A27" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B27" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="F27" s="11" t="s">
         <v>105</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>108</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>25</v>
@@ -2201,22 +2221,22 @@
     </row>
     <row r="28" spans="1:8" ht="39.6">
       <c r="A28" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B28" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="F28" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>45</v>
@@ -2225,22 +2245,22 @@
     </row>
     <row r="29" spans="1:8" ht="39.6">
       <c r="A29" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B29" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="F29" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>45</v>
@@ -2249,22 +2269,22 @@
     </row>
     <row r="30" spans="1:8" ht="39.6">
       <c r="A30" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B30" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="F30" s="11" t="s">
         <v>123</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>126</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>25</v>
@@ -2273,22 +2293,22 @@
     </row>
     <row r="31" spans="1:8" ht="52.8">
       <c r="A31" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B31" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F31" s="11" t="s">
         <v>128</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>25</v>
@@ -2296,22 +2316,22 @@
     </row>
     <row r="32" spans="1:8" ht="26.4">
       <c r="A32" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B32" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="F32" s="11" t="s">
         <v>134</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>137</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>25</v>
@@ -2320,22 +2340,22 @@
     </row>
     <row r="33" spans="1:8" ht="52.8">
       <c r="A33" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B33" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F33" s="11" t="s">
         <v>139</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>142</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>45</v>
@@ -2344,22 +2364,22 @@
     </row>
     <row r="34" spans="1:8" ht="39.6">
       <c r="A34" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B34" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F34" s="11" t="s">
         <v>144</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>147</v>
       </c>
       <c r="G34" s="12" t="s">
         <v>25</v>
@@ -2372,7 +2392,7 @@
         <v>4</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -2386,7 +2406,7 @@
         <v>17</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D36" s="27"/>
       <c r="E36" s="28"/>
@@ -2396,20 +2416,20 @@
     </row>
     <row r="37" spans="1:8" ht="26.4">
       <c r="A37" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G37" s="12" t="s">
         <v>25</v>
@@ -2418,22 +2438,22 @@
     </row>
     <row r="38" spans="1:8" ht="39.6">
       <c r="A38" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D38" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="E38" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="F38" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="D38" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>161</v>
       </c>
       <c r="G38" s="12" t="s">
         <v>25</v>
@@ -2442,22 +2462,22 @@
     </row>
     <row r="39" spans="1:8" ht="39.6">
       <c r="A39" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D39" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="D39" s="29" t="s">
-        <v>165</v>
-      </c>
       <c r="E39" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>25</v>
@@ -2466,22 +2486,22 @@
     </row>
     <row r="40" spans="1:8" ht="39.6">
       <c r="A40" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="D40" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="E40" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="F40" s="14" t="s">
         <v>168</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>171</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>25</v>
@@ -2490,22 +2510,22 @@
     </row>
     <row r="41" spans="1:8" ht="26.4">
       <c r="A41" s="8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D41" s="30" t="s">
         <v>32</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>45</v>
@@ -2514,22 +2534,22 @@
     </row>
     <row r="42" spans="1:8" ht="26.4">
       <c r="A42" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="D42" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="E42" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="F42" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>182</v>
       </c>
       <c r="G42" s="12" t="s">
         <v>25</v>
@@ -2538,22 +2558,22 @@
     </row>
     <row r="43" spans="1:8" ht="26.4">
       <c r="A43" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="D43" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="E43" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="F43" s="16" t="s">
         <v>185</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>188</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>25</v>
@@ -2562,22 +2582,22 @@
     </row>
     <row r="44" spans="1:8" ht="39.6">
       <c r="A44" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D44" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="E44" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="F44" s="14" t="s">
         <v>191</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>194</v>
       </c>
       <c r="G44" s="12" t="s">
         <v>25</v>
@@ -2586,22 +2606,22 @@
     </row>
     <row r="45" spans="1:8" ht="39.6">
       <c r="A45" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="D45" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="E45" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="F45" s="14" t="s">
         <v>197</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>200</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>25</v>
@@ -2610,22 +2630,22 @@
     </row>
     <row r="46" spans="1:8" ht="26.4">
       <c r="A46" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="D46" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="E46" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="F46" s="14" t="s">
         <v>203</v>
-      </c>
-      <c r="D46" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="E46" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>206</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>25</v>
@@ -2634,22 +2654,22 @@
     </row>
     <row r="47" spans="1:8" ht="26.4">
       <c r="A47" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D47" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="E47" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="F47" s="17" t="s">
         <v>209</v>
-      </c>
-      <c r="D47" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="E47" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>212</v>
       </c>
       <c r="G47" s="12" t="s">
         <v>25</v>
@@ -2662,7 +2682,7 @@
         <v>5</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D48" s="32"/>
       <c r="E48" s="9"/>
@@ -2672,46 +2692,46 @@
     </row>
     <row r="49" spans="1:8" ht="39.6">
       <c r="A49" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D49" s="11"/>
       <c r="E49" s="11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G49" s="12" t="s">
         <v>25</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="39.6">
       <c r="A50" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="D50" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="E50" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="F50" s="11" t="s">
         <v>222</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="E50" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>225</v>
       </c>
       <c r="G50" s="12" t="s">
         <v>25</v>
@@ -2720,22 +2740,22 @@
     </row>
     <row r="51" spans="1:8" ht="39.6">
       <c r="A51" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D51" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="E51" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="F51" s="11" t="s">
         <v>228</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="E51" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="F51" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="G51" s="12" t="s">
         <v>25</v>
@@ -2744,22 +2764,22 @@
     </row>
     <row r="52" spans="1:8" ht="39.6">
       <c r="A52" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D52" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="E52" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="F52" s="11" t="s">
         <v>234</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="E52" s="16" t="s">
-        <v>236</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>237</v>
       </c>
       <c r="G52" s="12" t="s">
         <v>25</v>
@@ -2768,22 +2788,22 @@
     </row>
     <row r="53" spans="1:8" ht="39.6">
       <c r="A53" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="D53" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="E53" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="F53" s="11" t="s">
         <v>240</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="E53" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="F53" s="11" t="s">
-        <v>243</v>
       </c>
       <c r="G53" s="12" t="s">
         <v>25</v>
@@ -2792,22 +2812,22 @@
     </row>
     <row r="54" spans="1:8" ht="39.6">
       <c r="A54" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D54" s="33">
         <v>12345678</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G54" s="12" t="s">
         <v>45</v>
@@ -2816,22 +2836,22 @@
     </row>
     <row r="55" spans="1:8" ht="39.6">
       <c r="A55" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="D55" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="E55" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="E55" s="16" t="s">
-        <v>253</v>
-      </c>
       <c r="F55" s="11" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G55" s="12" t="s">
         <v>45</v>
@@ -2840,22 +2860,22 @@
     </row>
     <row r="56" spans="1:8" ht="39.6">
       <c r="A56" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="D56" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="E56" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="C56" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="E56" s="16" t="s">
-        <v>258</v>
-      </c>
       <c r="F56" s="11" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G56" s="12" t="s">
         <v>45</v>
@@ -2864,22 +2884,22 @@
     </row>
     <row r="57" spans="1:8" ht="39.6">
       <c r="A57" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="E57" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="B57" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="E57" s="16" t="s">
-        <v>262</v>
-      </c>
       <c r="F57" s="11" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G57" s="12" t="s">
         <v>45</v>
@@ -2888,22 +2908,22 @@
     </row>
     <row r="58" spans="1:8" ht="39.6">
       <c r="A58" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D58" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="E58" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="C58" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>267</v>
-      </c>
       <c r="F58" s="11" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G58" s="12" t="s">
         <v>45</v>
@@ -2912,22 +2932,22 @@
     </row>
     <row r="59" spans="1:8" ht="26.4">
       <c r="A59" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="D59" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="E59" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="C59" s="17" t="s">
-        <v>270</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="E59" s="16" t="s">
-        <v>272</v>
-      </c>
       <c r="F59" s="11" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G59" s="12" t="s">
         <v>45</v>
@@ -2936,22 +2956,22 @@
     </row>
     <row r="60" spans="1:8" ht="26.4">
       <c r="A60" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="D60" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="E60" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="C60" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="E60" s="16" t="s">
-        <v>277</v>
-      </c>
       <c r="F60" s="11" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G60" s="12" t="s">
         <v>45</v>
@@ -2960,22 +2980,22 @@
     </row>
     <row r="61" spans="1:8" ht="26.4">
       <c r="A61" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="E61" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="F61" s="11" t="s">
         <v>279</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="E61" s="16" t="s">
-        <v>281</v>
-      </c>
-      <c r="F61" s="11" t="s">
-        <v>282</v>
       </c>
       <c r="G61" s="12" t="s">
         <v>45</v>

</xml_diff>